<commit_message>
update scripts sau khi nang cap he thong
</commit_message>
<xml_diff>
--- a/AAA/myRepo-master/cypress/fixtures/invalidBRN.xlsx
+++ b/AAA/myRepo-master/cypress/fixtures/invalidBRN.xlsx
@@ -399,7 +399,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,7 +417,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>100264</v>
+        <v>131887</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>

</xml_diff>